<commit_message>
plan van aanpak en logboek
</commit_message>
<xml_diff>
--- a/documentatie/logboek/personlijke_logboek/Logboek_Ben_Smits.xlsx
+++ b/documentatie/logboek/personlijke_logboek/Logboek_Ben_Smits.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="18">
   <si>
     <t xml:space="preserve">Project Fifa </t>
   </si>
@@ -449,7 +449,7 @@
   <dimension ref="A1:P42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -606,28 +606,42 @@
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
+        <v>42989</v>
+      </c>
+      <c r="C17" s="4">
+        <v>0.40972222222222227</v>
+      </c>
+      <c r="E17" t="s">
+        <v>10</v>
+      </c>
+      <c r="G17" t="s">
+        <v>11</v>
+      </c>
+      <c r="I17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
sale backend + logboek
</commit_message>
<xml_diff>
--- a/documentatie/logboek/personlijke_logboek/Logboek_Ben_Smits.xlsx
+++ b/documentatie/logboek/personlijke_logboek/Logboek_Ben_Smits.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="34">
   <si>
     <t xml:space="preserve">Project Fifa </t>
   </si>
@@ -123,6 +123,9 @@
   </si>
   <si>
     <t>back end van sales</t>
+  </si>
+  <si>
+    <t>database connection sales</t>
   </si>
 </sst>
 </file>
@@ -499,10 +502,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P42"/>
+  <dimension ref="A1:P43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="I41" sqref="I41"/>
+      <selection activeCell="N46" sqref="N46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -933,6 +936,23 @@
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
     </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="4">
+        <v>43017</v>
+      </c>
+      <c r="C43" s="5">
+        <v>0.375</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I43" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
login backend + logboek
</commit_message>
<xml_diff>
--- a/documentatie/logboek/personlijke_logboek/Logboek_Ben_Smits.xlsx
+++ b/documentatie/logboek/personlijke_logboek/Logboek_Ben_Smits.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="37">
   <si>
     <t xml:space="preserve">Project Fifa </t>
   </si>
@@ -132,6 +132,9 @@
   </si>
   <si>
     <t>sales create connectie</t>
+  </si>
+  <si>
+    <t>login backend</t>
   </si>
 </sst>
 </file>
@@ -508,10 +511,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P47"/>
+  <dimension ref="A1:P49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="I47" sqref="I47"/>
+      <selection activeCell="I49" sqref="I49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -993,6 +996,23 @@
         <v>35</v>
       </c>
     </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" s="4">
+        <v>43020</v>
+      </c>
+      <c r="C49" s="5">
+        <v>0.375</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I49" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>